<commit_message>
Added Keras TF files
</commit_message>
<xml_diff>
--- a/Classification Cont.xlsx
+++ b/Classification Cont.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whatch2\Desktop\ClassificationCompetition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Documents\SCHOOL\Towson\2018-2022 -- DSc - Computer Security\6_Fall 2018\COSC 757 - Data Mining\Assignments\Classification Competition - 11-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9485DF9-9BBE-4092-B870-4D255A4A36DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Learning" sheetId="3" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Sheet5" sheetId="7" r:id="rId4"/>
     <sheet name="crossval" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="80">
   <si>
     <t>TN</t>
   </si>
@@ -263,19 +264,19 @@
     <t>RF-100-entropy</t>
   </si>
   <si>
-    <t>RF-2000</t>
-  </si>
-  <si>
     <t>FULL SET RF min-max</t>
   </si>
   <si>
     <t>Numeric Only min-max 1</t>
   </si>
+  <si>
+    <t>RF-250-entropy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -3302,11 +3303,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,7 +3498,7 @@
       </c>
       <c r="S6" s="19">
         <f>B69</f>
-        <v>0.94522636397025706</v>
+        <v>0.94267617443850704</v>
       </c>
       <c r="T6" s="19">
         <f>B76</f>
@@ -3569,7 +3570,7 @@
       </c>
       <c r="S7" s="18">
         <f t="shared" ref="S7:S10" si="10">B70</f>
-        <v>0.94267617443850704</v>
+        <v>0.94284942100995806</v>
       </c>
       <c r="T7" s="18">
         <f t="shared" ref="T7:T10" si="11">B77</f>
@@ -3641,7 +3642,7 @@
       </c>
       <c r="S8" s="18">
         <f t="shared" si="10"/>
-        <v>0.94284942100995806</v>
+        <v>0.94316819470142599</v>
       </c>
       <c r="T8" s="18">
         <f t="shared" si="11"/>
@@ -3713,7 +3714,7 @@
       </c>
       <c r="S9" s="18">
         <f t="shared" si="10"/>
-        <v>0.94316819470142599</v>
+        <v>0.94522636397025706</v>
       </c>
       <c r="T9" s="18">
         <f t="shared" si="11"/>
@@ -3785,7 +3786,7 @@
       </c>
       <c r="S10" s="17">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.950680166039514</v>
       </c>
       <c r="T10" s="17">
         <f t="shared" si="11"/>
@@ -3928,7 +3929,7 @@
       </c>
       <c r="S13" s="19">
         <f>C69</f>
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="T13" s="19">
         <f>C76</f>
@@ -4144,7 +4145,7 @@
       </c>
       <c r="S16" s="18">
         <f t="shared" si="24"/>
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="T16" s="18">
         <f t="shared" si="25"/>
@@ -4216,7 +4217,7 @@
       </c>
       <c r="S17" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="T17" s="17">
         <f t="shared" si="25"/>
@@ -4364,7 +4365,7 @@
       </c>
       <c r="S20" s="19">
         <f>D69</f>
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="T20" s="19">
         <f>D76</f>
@@ -4580,7 +4581,7 @@
       </c>
       <c r="S23" s="18">
         <f t="shared" si="38"/>
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="T23" s="18">
         <f t="shared" si="39"/>
@@ -4652,7 +4653,7 @@
       </c>
       <c r="S24" s="17">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="T24" s="17">
         <f t="shared" si="39"/>
@@ -5083,7 +5084,7 @@
       </c>
       <c r="S31" s="17">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="T31" s="17">
         <f t="shared" si="53"/>
@@ -5702,7 +5703,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -5722,16 +5723,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B69">
-        <v>0.94522636397025706</v>
+        <v>0.94267617443850704</v>
       </c>
       <c r="C69">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="D69">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="E69">
         <v>0.94</v>
@@ -5742,10 +5743,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70">
-        <v>0.94267617443850704</v>
+        <v>0.94284942100995806</v>
       </c>
       <c r="C70">
         <v>0.94</v>
@@ -5762,10 +5763,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B71">
-        <v>0.94284942100995806</v>
+        <v>0.94316819470142599</v>
       </c>
       <c r="C71">
         <v>0.94</v>
@@ -5782,16 +5783,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B72">
-        <v>0.94316819470142599</v>
+        <v>0.94522636397025706</v>
       </c>
       <c r="C72">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="D72">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="E72">
         <v>0.94</v>
@@ -5802,7 +5803,19 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="B73">
+        <v>0.950680166039514</v>
+      </c>
+      <c r="C73">
+        <v>0.95</v>
+      </c>
+      <c r="D73">
+        <v>0.95</v>
+      </c>
+      <c r="E73">
+        <v>0.95</v>
       </c>
       <c r="F73">
         <v>144303</v>
@@ -5810,7 +5823,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -6077,16 +6090,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6178,9 +6191,9 @@
         <f>A29</f>
         <v>Numeric Only 1</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="27" t="str">
         <f>A37</f>
-        <v>0</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="O5" s="27">
         <f>A45</f>
@@ -6244,7 +6257,7 @@
       </c>
       <c r="L6" s="19">
         <f>B22</f>
-        <v>0.64297772196951397</v>
+        <v>0.64724470562146497</v>
       </c>
       <c r="M6" s="19">
         <f>B30</f>
@@ -6252,7 +6265,7 @@
       </c>
       <c r="N6" s="19">
         <f>B38</f>
-        <v>0</v>
+        <v>0.66467318993236502</v>
       </c>
       <c r="O6" s="19">
         <f>B46</f>
@@ -6316,7 +6329,7 @@
       </c>
       <c r="L7" s="18">
         <f t="shared" ref="L7:L10" si="2">B23</f>
-        <v>0.64948899403756999</v>
+        <v>0.65204706730236095</v>
       </c>
       <c r="M7" s="18">
         <f t="shared" ref="M7:M10" si="3">B31</f>
@@ -6324,7 +6337,7 @@
       </c>
       <c r="N7" s="18">
         <f t="shared" ref="N7:N10" si="4">B39</f>
-        <v>0</v>
+        <v>0.803803082381638</v>
       </c>
       <c r="O7" s="18">
         <f t="shared" ref="O7:O10" si="5">B47</f>
@@ -6388,7 +6401,7 @@
       </c>
       <c r="L8" s="18">
         <f t="shared" si="2"/>
-        <v>0.65057004814848696</v>
+        <v>0.65145803304135697</v>
       </c>
       <c r="M8" s="18">
         <f t="shared" si="3"/>
@@ -6396,7 +6409,7 @@
       </c>
       <c r="N8" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.74379088590752795</v>
       </c>
       <c r="O8" s="18">
         <f t="shared" si="5"/>
@@ -6701,9 +6714,9 @@
         <f t="shared" si="24"/>
         <v>Numeric Only 1</v>
       </c>
-      <c r="N13" s="27">
+      <c r="N13" s="27" t="str">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="O13" s="27">
         <f t="shared" si="24"/>
@@ -6775,7 +6788,7 @@
       </c>
       <c r="N14" s="19">
         <f>C38</f>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="O14" s="19">
         <f>C46</f>
@@ -6847,7 +6860,7 @@
       </c>
       <c r="N15" s="18">
         <f t="shared" ref="N15:N18" si="30">C39</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="O15" s="18">
         <f t="shared" ref="O15:O18" si="31">C47</f>
@@ -6919,7 +6932,7 @@
       </c>
       <c r="N16" s="18">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="O16" s="18">
         <f t="shared" si="31"/>
@@ -7188,9 +7201,9 @@
         <f t="shared" si="50"/>
         <v>Numeric Only 1</v>
       </c>
-      <c r="N21" s="27">
+      <c r="N21" s="27" t="str">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="O21" s="27">
         <f t="shared" si="50"/>
@@ -7226,13 +7239,13 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.64297772196951397</v>
+        <v>0.64724470562146497</v>
       </c>
       <c r="C22">
         <v>0.63</v>
       </c>
       <c r="D22">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="E22">
         <v>0.62</v>
@@ -7254,7 +7267,7 @@
       </c>
       <c r="L22" s="19">
         <f>D22</f>
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="M22" s="19">
         <f>D30</f>
@@ -7262,7 +7275,7 @@
       </c>
       <c r="N22" s="19">
         <f>D38</f>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="O22" s="19">
         <f>D46</f>
@@ -7298,7 +7311,7 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.64948899403756999</v>
+        <v>0.65204706730236095</v>
       </c>
       <c r="C23">
         <v>0.64</v>
@@ -7307,7 +7320,7 @@
         <v>0.65</v>
       </c>
       <c r="E23">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="F23">
         <v>120253</v>
@@ -7334,7 +7347,7 @@
       </c>
       <c r="N23" s="18">
         <f t="shared" ref="N23:N26" si="56">D39</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="O23" s="18">
         <f t="shared" ref="O23:O26" si="57">D47</f>
@@ -7370,7 +7383,7 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.65057004814848696</v>
+        <v>0.65145803304135697</v>
       </c>
       <c r="C24">
         <v>0.64</v>
@@ -7406,7 +7419,7 @@
       </c>
       <c r="N24" s="18">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="O24" s="18">
         <f t="shared" si="57"/>
@@ -7669,9 +7682,9 @@
         <f t="shared" si="75"/>
         <v>Numeric Only 1</v>
       </c>
-      <c r="N29" s="27">
+      <c r="N29" s="27" t="str">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="O29" s="27">
         <f t="shared" si="75"/>
@@ -7731,7 +7744,7 @@
       </c>
       <c r="N30" s="19">
         <f>E38</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="O30" s="19">
         <f>E46</f>
@@ -7783,7 +7796,7 @@
       </c>
       <c r="L31" s="18">
         <f t="shared" si="78"/>
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="M31" s="18">
         <f t="shared" ref="M31:M34" si="80">E31</f>
@@ -7791,7 +7804,7 @@
       </c>
       <c r="N31" s="18">
         <f t="shared" ref="N31:N34" si="81">E39</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="O31" s="18">
         <f t="shared" ref="O31:O34" si="82">E47</f>
@@ -7851,7 +7864,7 @@
       </c>
       <c r="N32" s="18">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="O32" s="18">
         <f t="shared" si="82"/>
@@ -8063,7 +8076,9 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
@@ -8084,6 +8099,18 @@
       <c r="A38" t="s">
         <v>27</v>
       </c>
+      <c r="B38">
+        <v>0.66467318993236502</v>
+      </c>
+      <c r="C38">
+        <v>0.64</v>
+      </c>
+      <c r="D38">
+        <v>0.65</v>
+      </c>
+      <c r="E38">
+        <v>0.63</v>
+      </c>
       <c r="F38">
         <v>120253</v>
       </c>
@@ -8092,6 +8119,18 @@
       <c r="A39" t="s">
         <v>28</v>
       </c>
+      <c r="B39">
+        <v>0.803803082381638</v>
+      </c>
+      <c r="C39">
+        <v>0.8</v>
+      </c>
+      <c r="D39">
+        <v>0.8</v>
+      </c>
+      <c r="E39">
+        <v>0.8</v>
+      </c>
       <c r="F39">
         <v>120253</v>
       </c>
@@ -8099,6 +8138,18 @@
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
+      </c>
+      <c r="B40">
+        <v>0.74379088590752795</v>
+      </c>
+      <c r="C40">
+        <v>0.74</v>
+      </c>
+      <c r="D40">
+        <v>0.74</v>
+      </c>
+      <c r="E40">
+        <v>0.74</v>
       </c>
       <c r="F40">
         <v>120253</v>
@@ -8741,7 +8792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8850,7 +8901,7 @@
       </c>
       <c r="K4" s="19">
         <f>'Basic Learning'!S6</f>
-        <v>0.94522636397025706</v>
+        <v>0.94267617443850704</v>
       </c>
       <c r="L4" s="19">
         <f>'Basic Learning'!T6</f>
@@ -8903,7 +8954,7 @@
       </c>
       <c r="K5" s="18">
         <f>'Basic Learning'!S7</f>
-        <v>0.94267617443850704</v>
+        <v>0.94284942100995806</v>
       </c>
       <c r="L5" s="18">
         <f>'Basic Learning'!T7</f>
@@ -8956,7 +9007,7 @@
       </c>
       <c r="K6" s="18">
         <f>'Basic Learning'!S8</f>
-        <v>0.94284942100995806</v>
+        <v>0.94316819470142599</v>
       </c>
       <c r="L6" s="18">
         <f>'Basic Learning'!T8</f>
@@ -9009,7 +9060,7 @@
       </c>
       <c r="K7" s="18">
         <f>'Basic Learning'!S9</f>
-        <v>0.94316819470142599</v>
+        <v>0.94522636397025706</v>
       </c>
       <c r="L7" s="18">
         <f>'Basic Learning'!T9</f>
@@ -9062,7 +9113,7 @@
       </c>
       <c r="K8" s="17">
         <f>'Basic Learning'!S10</f>
-        <v>0</v>
+        <v>0.950680166039514</v>
       </c>
       <c r="L8" s="17">
         <f>'Basic Learning'!T10</f>
@@ -9087,7 +9138,7 @@
       </c>
       <c r="D9" s="19">
         <f>'Advanced Learning'!L6</f>
-        <v>0.64297772196951397</v>
+        <v>0.64724470562146497</v>
       </c>
       <c r="E9" s="19">
         <f>'Advanced Learning'!M6</f>
@@ -9095,7 +9146,7 @@
       </c>
       <c r="F9" s="19">
         <f>'Advanced Learning'!N6</f>
-        <v>0</v>
+        <v>0.66467318993236502</v>
       </c>
       <c r="G9" s="19">
         <f>'Advanced Learning'!O6</f>
@@ -9140,7 +9191,7 @@
       </c>
       <c r="D10" s="18">
         <f>'Advanced Learning'!L7</f>
-        <v>0.64948899403756999</v>
+        <v>0.65204706730236095</v>
       </c>
       <c r="E10" s="18">
         <f>'Advanced Learning'!M7</f>
@@ -9148,7 +9199,7 @@
       </c>
       <c r="F10" s="18">
         <f>'Advanced Learning'!N7</f>
-        <v>0</v>
+        <v>0.803803082381638</v>
       </c>
       <c r="G10" s="18">
         <f>'Advanced Learning'!O7</f>
@@ -9193,7 +9244,7 @@
       </c>
       <c r="D11" s="18">
         <f>'Advanced Learning'!L8</f>
-        <v>0.65057004814848696</v>
+        <v>0.65145803304135697</v>
       </c>
       <c r="E11" s="18">
         <f>'Advanced Learning'!M8</f>
@@ -9201,7 +9252,7 @@
       </c>
       <c r="F11" s="18">
         <f>'Advanced Learning'!N8</f>
-        <v>0</v>
+        <v>0.74379088590752795</v>
       </c>
       <c r="G11" s="18">
         <f>'Advanced Learning'!O8</f>
@@ -9486,7 +9537,7 @@
       </c>
       <c r="K18" s="6">
         <f>'Basic Learning'!S13</f>
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="L18" s="6">
         <f>'Basic Learning'!T13</f>
@@ -9645,7 +9696,7 @@
       </c>
       <c r="K21" s="9">
         <f>'Basic Learning'!S16</f>
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="L21" s="9">
         <f>'Basic Learning'!T16</f>
@@ -9698,7 +9749,7 @@
       </c>
       <c r="K22" s="12">
         <f>'Basic Learning'!S17</f>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="L22" s="12">
         <f>'Basic Learning'!T17</f>
@@ -9731,7 +9782,7 @@
       </c>
       <c r="F23" s="6">
         <f>'Advanced Learning'!N14</f>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="G23" s="6">
         <f>'Advanced Learning'!O14</f>
@@ -9784,7 +9835,7 @@
       </c>
       <c r="F24" s="9">
         <f>'Advanced Learning'!N15</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G24" s="9">
         <f>'Advanced Learning'!O15</f>
@@ -9837,7 +9888,7 @@
       </c>
       <c r="F25" s="9">
         <f>'Advanced Learning'!N16</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="G25" s="9">
         <f>'Advanced Learning'!O16</f>
@@ -10122,7 +10173,7 @@
       </c>
       <c r="K32" s="6">
         <f>'Basic Learning'!S20</f>
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="L32" s="6">
         <f>'Basic Learning'!T20</f>
@@ -10281,7 +10332,7 @@
       </c>
       <c r="K35" s="9">
         <f>'Basic Learning'!S23</f>
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="L35" s="9">
         <f>'Basic Learning'!T23</f>
@@ -10334,7 +10385,7 @@
       </c>
       <c r="K36" s="12">
         <f>'Basic Learning'!S24</f>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="L36" s="12">
         <f>'Basic Learning'!T24</f>
@@ -10359,7 +10410,7 @@
       </c>
       <c r="D37" s="6">
         <f>'Advanced Learning'!L22</f>
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="E37" s="6">
         <f>'Advanced Learning'!M22</f>
@@ -10367,7 +10418,7 @@
       </c>
       <c r="F37" s="6">
         <f>'Advanced Learning'!N22</f>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="G37" s="6">
         <f>'Advanced Learning'!O22</f>
@@ -10420,7 +10471,7 @@
       </c>
       <c r="F38" s="9">
         <f>'Advanced Learning'!N23</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G38" s="9">
         <f>'Advanced Learning'!O23</f>
@@ -10473,7 +10524,7 @@
       </c>
       <c r="F39" s="9">
         <f>'Advanced Learning'!N24</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="G39" s="9">
         <f>'Advanced Learning'!O24</f>
@@ -10970,7 +11021,7 @@
       </c>
       <c r="K50" s="12">
         <f>'Basic Learning'!S31</f>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="L50" s="12">
         <f>'Basic Learning'!T31</f>
@@ -11003,7 +11054,7 @@
       </c>
       <c r="F51" s="6">
         <f>'Advanced Learning'!N30</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="G51" s="6">
         <f>'Advanced Learning'!O30</f>
@@ -11048,7 +11099,7 @@
       </c>
       <c r="D52" s="9">
         <f>'Advanced Learning'!L31</f>
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="E52" s="9">
         <f>'Advanced Learning'!M31</f>
@@ -11056,7 +11107,7 @@
       </c>
       <c r="F52" s="9">
         <f>'Advanced Learning'!N31</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G52" s="9">
         <f>'Advanced Learning'!O31</f>
@@ -11109,7 +11160,7 @@
       </c>
       <c r="F53" s="9">
         <f>'Advanced Learning'!N32</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="G53" s="9">
         <f>'Advanced Learning'!O32</f>
@@ -11449,7 +11500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11713,7 +11764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">

</xml_diff>

<commit_message>
updated xls, added RNN file
</commit_message>
<xml_diff>
--- a/Classification Cont.xlsx
+++ b/Classification Cont.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Documents\SCHOOL\Towson\2018-2022 -- DSc - Computer Security\6_Fall 2018\COSC 757 - Data Mining\Assignments\Classification Competition - 11-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CAFA98-3256-48F6-9C84-7C153C6B57EA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBBAFDE-8F7B-4FFD-9BA0-AD389C31B201}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="87">
   <si>
     <t>TN</t>
   </si>
@@ -271,6 +271,27 @@
   </si>
   <si>
     <t>RF-250-entropy</t>
+  </si>
+  <si>
+    <t>Deep Networks</t>
+  </si>
+  <si>
+    <t>250-100-10-7</t>
+  </si>
+  <si>
+    <t>250-100-10-7_32-16</t>
+  </si>
+  <si>
+    <t>250-100-10-7_1-64</t>
+  </si>
+  <si>
+    <t>250-100-10-7_1-64-bin</t>
+  </si>
+  <si>
+    <t>250-100-10-7_1-64-mult</t>
+  </si>
+  <si>
+    <t>250-100-10-7_RNN</t>
   </si>
 </sst>
 </file>
@@ -6093,8 +6114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6195,9 +6216,9 @@
         <f>A37</f>
         <v>Numeric Only min-max 1</v>
       </c>
-      <c r="O5" s="27">
+      <c r="O5" s="27" t="str">
         <f>A45</f>
-        <v>0</v>
+        <v>Deep Networks</v>
       </c>
       <c r="P5" s="27">
         <f>A53</f>
@@ -6261,7 +6282,7 @@
       </c>
       <c r="M6" s="19">
         <f>B30</f>
-        <v>0</v>
+        <v>0.65996091584432803</v>
       </c>
       <c r="N6" s="19">
         <f>B38</f>
@@ -6269,7 +6290,7 @@
       </c>
       <c r="O6" s="19">
         <f>B46</f>
-        <v>0</v>
+        <v>0.93721587857142852</v>
       </c>
       <c r="P6" s="19">
         <f>B54</f>
@@ -6333,7 +6354,7 @@
       </c>
       <c r="M7" s="18">
         <f t="shared" ref="M7:M10" si="3">B31</f>
-        <v>0</v>
+        <v>0.48720756181394798</v>
       </c>
       <c r="N7" s="18">
         <f t="shared" ref="N7:N10" si="4">B39</f>
@@ -6341,7 +6362,7 @@
       </c>
       <c r="O7" s="18">
         <f t="shared" ref="O7:O10" si="5">B47</f>
-        <v>0</v>
+        <v>0.89939790000000008</v>
       </c>
       <c r="P7" s="18">
         <f t="shared" ref="P7:P10" si="6">B55</f>
@@ -6405,7 +6426,7 @@
       </c>
       <c r="M8" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.48079055327641601</v>
       </c>
       <c r="N8" s="18">
         <f t="shared" si="4"/>
@@ -6413,7 +6434,7 @@
       </c>
       <c r="O8" s="18">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.91746491571428568</v>
       </c>
       <c r="P8" s="18">
         <f t="shared" si="6"/>
@@ -6485,7 +6506,7 @@
       </c>
       <c r="O9" s="18">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.96847132285714288</v>
       </c>
       <c r="P9" s="18">
         <f t="shared" si="6"/>
@@ -6718,9 +6739,9 @@
         <f t="shared" si="24"/>
         <v>Numeric Only min-max 1</v>
       </c>
-      <c r="O13" s="27">
+      <c r="O13" s="27" t="str">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>Deep Networks</v>
       </c>
       <c r="P13" s="27">
         <f t="shared" si="24"/>
@@ -6784,7 +6805,7 @@
       </c>
       <c r="M14" s="19">
         <f>C30</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="N14" s="19">
         <f>C38</f>
@@ -6792,7 +6813,7 @@
       </c>
       <c r="O14" s="19">
         <f>C46</f>
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="P14" s="19">
         <f>C54</f>
@@ -6856,7 +6877,7 @@
       </c>
       <c r="M15" s="18">
         <f t="shared" ref="M15:M18" si="29">C31</f>
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" ref="N15:N18" si="30">C39</f>
@@ -6864,7 +6885,7 @@
       </c>
       <c r="O15" s="18">
         <f t="shared" ref="O15:O18" si="31">C47</f>
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="P15" s="18">
         <f t="shared" ref="P15:P18" si="32">C55</f>
@@ -6928,7 +6949,7 @@
       </c>
       <c r="M16" s="18">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="30"/>
@@ -6936,7 +6957,7 @@
       </c>
       <c r="O16" s="18">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="P16" s="18">
         <f t="shared" si="32"/>
@@ -6996,7 +7017,7 @@
       </c>
       <c r="O17" s="18">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P17" s="18">
         <f t="shared" si="32"/>
@@ -7205,9 +7226,9 @@
         <f t="shared" si="50"/>
         <v>Numeric Only min-max 1</v>
       </c>
-      <c r="O21" s="27">
+      <c r="O21" s="27" t="str">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>Deep Networks</v>
       </c>
       <c r="P21" s="27">
         <f t="shared" si="50"/>
@@ -7250,8 +7271,8 @@
       <c r="E22">
         <v>0.62</v>
       </c>
-      <c r="F22">
-        <v>120253</v>
+      <c r="F22" s="1">
+        <v>144304</v>
       </c>
       <c r="I22" s="5" t="str">
         <f>A22</f>
@@ -7271,7 +7292,7 @@
       </c>
       <c r="M22" s="19">
         <f>D30</f>
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="N22" s="19">
         <f>D38</f>
@@ -7279,7 +7300,7 @@
       </c>
       <c r="O22" s="19">
         <f>D46</f>
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="P22" s="19">
         <f>D54</f>
@@ -7322,8 +7343,8 @@
       <c r="E23">
         <v>0.63</v>
       </c>
-      <c r="F23">
-        <v>120253</v>
+      <c r="F23" s="1">
+        <v>144304</v>
       </c>
       <c r="I23" s="8" t="str">
         <f t="shared" ref="I23:I26" si="53">A23</f>
@@ -7343,7 +7364,7 @@
       </c>
       <c r="M23" s="18">
         <f t="shared" ref="M23:M26" si="55">D31</f>
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="N23" s="18">
         <f t="shared" ref="N23:N26" si="56">D39</f>
@@ -7351,7 +7372,7 @@
       </c>
       <c r="O23" s="18">
         <f t="shared" ref="O23:O26" si="57">D47</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="P23" s="18">
         <f t="shared" ref="P23:P26" si="58">D55</f>
@@ -7394,8 +7415,8 @@
       <c r="E24">
         <v>0.63</v>
       </c>
-      <c r="F24">
-        <v>120253</v>
+      <c r="F24" s="1">
+        <v>144304</v>
       </c>
       <c r="I24" s="8" t="str">
         <f t="shared" si="53"/>
@@ -7415,7 +7436,7 @@
       </c>
       <c r="M24" s="18">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="56"/>
@@ -7423,7 +7444,7 @@
       </c>
       <c r="O24" s="18">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P24" s="18">
         <f t="shared" si="58"/>
@@ -7466,8 +7487,8 @@
       <c r="E25">
         <v>0.63</v>
       </c>
-      <c r="F25">
-        <v>120253</v>
+      <c r="F25" s="1">
+        <v>144304</v>
       </c>
       <c r="I25" s="8" t="str">
         <f t="shared" si="53"/>
@@ -7495,7 +7516,7 @@
       </c>
       <c r="O25" s="18">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="P25" s="18">
         <f t="shared" si="58"/>
@@ -7538,8 +7559,8 @@
       <c r="E26">
         <v>0.12</v>
       </c>
-      <c r="F26">
-        <v>120253</v>
+      <c r="F26" s="1">
+        <v>144304</v>
       </c>
       <c r="I26" s="8" t="str">
         <f t="shared" si="53"/>
@@ -7610,8 +7631,8 @@
       <c r="E27">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F27">
-        <v>120253</v>
+      <c r="F27" s="1">
+        <v>144304</v>
       </c>
       <c r="I27" s="11" t="str">
         <f t="shared" ref="I27" si="64">A27</f>
@@ -7722,9 +7743,9 @@
         <f t="shared" si="75"/>
         <v>Numeric Only min-max 1</v>
       </c>
-      <c r="O29" s="27">
+      <c r="O29" s="27" t="str">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>Deep Networks</v>
       </c>
       <c r="P29" s="27">
         <f t="shared" si="75"/>
@@ -7755,8 +7776,20 @@
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="F30">
-        <v>120253</v>
+      <c r="B30">
+        <v>0.65996091584432803</v>
+      </c>
+      <c r="C30">
+        <v>0.63</v>
+      </c>
+      <c r="D30">
+        <v>0.66</v>
+      </c>
+      <c r="E30">
+        <v>0.63</v>
+      </c>
+      <c r="F30" s="1">
+        <v>144304</v>
       </c>
       <c r="I30" s="5" t="str">
         <f>A30</f>
@@ -7776,7 +7809,7 @@
       </c>
       <c r="M30" s="19">
         <f>E30</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="N30" s="19">
         <f>E38</f>
@@ -7784,7 +7817,7 @@
       </c>
       <c r="O30" s="19">
         <f>E46</f>
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="P30" s="19">
         <f>E54</f>
@@ -7815,8 +7848,20 @@
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="F31">
-        <v>120253</v>
+      <c r="B31">
+        <v>0.48720756181394798</v>
+      </c>
+      <c r="C31">
+        <v>0.24</v>
+      </c>
+      <c r="D31">
+        <v>0.49</v>
+      </c>
+      <c r="E31">
+        <v>0.32</v>
+      </c>
+      <c r="F31" s="1">
+        <v>144304</v>
       </c>
       <c r="I31" s="8" t="str">
         <f t="shared" ref="I31:I34" si="79">A31</f>
@@ -7836,7 +7881,7 @@
       </c>
       <c r="M31" s="18">
         <f t="shared" ref="M31:M34" si="80">E31</f>
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="N31" s="18">
         <f t="shared" ref="N31:N34" si="81">E39</f>
@@ -7844,7 +7889,7 @@
       </c>
       <c r="O31" s="18">
         <f t="shared" ref="O31:O34" si="82">E47</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="P31" s="18">
         <f t="shared" ref="P31:P34" si="83">E55</f>
@@ -7875,8 +7920,20 @@
       <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="F32">
-        <v>120253</v>
+      <c r="B32">
+        <v>0.48079055327641601</v>
+      </c>
+      <c r="C32">
+        <v>0.37</v>
+      </c>
+      <c r="D32">
+        <v>0.48</v>
+      </c>
+      <c r="E32">
+        <v>0.33</v>
+      </c>
+      <c r="F32" s="1">
+        <v>144304</v>
       </c>
       <c r="I32" s="8" t="str">
         <f t="shared" si="79"/>
@@ -7896,7 +7953,7 @@
       </c>
       <c r="M32" s="18">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="N32" s="18">
         <f t="shared" si="81"/>
@@ -7904,7 +7961,7 @@
       </c>
       <c r="O32" s="18">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="P32" s="18">
         <f t="shared" si="83"/>
@@ -7935,8 +7992,8 @@
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="F33">
-        <v>120253</v>
+      <c r="F33" s="1">
+        <v>144304</v>
       </c>
       <c r="I33" s="8" t="str">
         <f t="shared" si="79"/>
@@ -7964,7 +8021,7 @@
       </c>
       <c r="O33" s="18">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="P33" s="18">
         <f t="shared" si="83"/>
@@ -7995,8 +8052,8 @@
       <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="F34">
-        <v>120253</v>
+      <c r="F34" s="1">
+        <v>144304</v>
       </c>
       <c r="I34" s="8" t="str">
         <f t="shared" si="79"/>
@@ -8055,8 +8112,8 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="F35">
-        <v>120253</v>
+      <c r="F35" s="1">
+        <v>144304</v>
       </c>
       <c r="I35" s="11" t="str">
         <f t="shared" ref="I35" si="89">A35</f>
@@ -8147,8 +8204,8 @@
       <c r="E38">
         <v>0.63</v>
       </c>
-      <c r="F38">
-        <v>120253</v>
+      <c r="F38" s="1">
+        <v>144304</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -8167,8 +8224,8 @@
       <c r="E39">
         <v>0.8</v>
       </c>
-      <c r="F39">
-        <v>120253</v>
+      <c r="F39" s="1">
+        <v>144304</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -8187,8 +8244,8 @@
       <c r="E40">
         <v>0.74</v>
       </c>
-      <c r="F40">
-        <v>120253</v>
+      <c r="F40" s="1">
+        <v>144304</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -8207,8 +8264,8 @@
       <c r="E41">
         <v>0.74</v>
       </c>
-      <c r="F41">
-        <v>120253</v>
+      <c r="F41" s="1">
+        <v>144304</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -8227,8 +8284,8 @@
       <c r="E42">
         <v>0.64</v>
       </c>
-      <c r="F42">
-        <v>120253</v>
+      <c r="F42" s="1">
+        <v>144304</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -8247,12 +8304,14 @@
       <c r="E43">
         <v>0.61</v>
       </c>
-      <c r="F43">
-        <v>120253</v>
+      <c r="F43" s="1">
+        <v>144304</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="B45" t="s">
         <v>6</v>
       </c>
@@ -8271,7 +8330,20 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>83</v>
+      </c>
+      <c r="B46">
+        <f>AVERAGE(0.83687909, 0.81979017, 0.96844162, 0.99526694, 0.98501774, 0.97060373, 0.98451186)</f>
+        <v>0.93721587857142852</v>
+      </c>
+      <c r="C46">
+        <v>0.78</v>
+      </c>
+      <c r="D46">
+        <v>0.77</v>
+      </c>
+      <c r="E46">
+        <v>0.76</v>
       </c>
       <c r="F46">
         <v>120253</v>
@@ -8279,7 +8351,20 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>84</v>
+      </c>
+      <c r="B47">
+        <f>AVERAGE(0.72299451, 0.69590587,0.95264858, 0.99526694,0.98354169, 0.97014636, 0.97528135)</f>
+        <v>0.89939790000000008</v>
+      </c>
+      <c r="C47">
+        <v>0.62</v>
+      </c>
+      <c r="D47">
+        <v>0.63</v>
+      </c>
+      <c r="E47">
+        <v>0.61</v>
       </c>
       <c r="F47">
         <v>120253</v>
@@ -8287,7 +8372,20 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>85</v>
+      </c>
+      <c r="B48">
+        <f>AVERAGE(0.77954873, 0.76406752, 0.95583629, 0.99526694,0.98354169,0.97014636, 0.97384688)</f>
+        <v>0.91746491571428568</v>
+      </c>
+      <c r="C48">
+        <v>0.69</v>
+      </c>
+      <c r="D48">
+        <v>0.7</v>
+      </c>
+      <c r="E48">
+        <v>0.69</v>
       </c>
       <c r="F48">
         <v>120253</v>
@@ -8295,7 +8393,20 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>82</v>
+      </c>
+      <c r="B49">
+        <f>AVERAGE(0.92409774,0.91172109,0.98151125,0.99745676,0.99081107,0.98283485, 0.9908665)</f>
+        <v>0.96847132285714288</v>
+      </c>
+      <c r="C49">
+        <v>0.9</v>
+      </c>
+      <c r="D49">
+        <v>0.88</v>
+      </c>
+      <c r="E49">
+        <v>0.89</v>
       </c>
       <c r="F49">
         <v>120253</v>
@@ -8303,7 +8414,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="F50">
         <v>120253</v>
@@ -8311,7 +8422,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="F51">
         <v>120253</v>
@@ -9214,7 +9325,7 @@
       </c>
       <c r="E9" s="19">
         <f>'Advanced Learning'!M6</f>
-        <v>0</v>
+        <v>0.65996091584432803</v>
       </c>
       <c r="F9" s="19">
         <f>'Advanced Learning'!N6</f>
@@ -9222,7 +9333,7 @@
       </c>
       <c r="G9" s="19">
         <f>'Advanced Learning'!O6</f>
-        <v>0</v>
+        <v>0.93721587857142852</v>
       </c>
       <c r="H9" s="19">
         <f>'Advanced Learning'!P6</f>
@@ -9267,7 +9378,7 @@
       </c>
       <c r="E10" s="18">
         <f>'Advanced Learning'!M7</f>
-        <v>0</v>
+        <v>0.48720756181394798</v>
       </c>
       <c r="F10" s="18">
         <f>'Advanced Learning'!N7</f>
@@ -9275,7 +9386,7 @@
       </c>
       <c r="G10" s="18">
         <f>'Advanced Learning'!O7</f>
-        <v>0</v>
+        <v>0.89939790000000008</v>
       </c>
       <c r="H10" s="18">
         <f>'Advanced Learning'!P7</f>
@@ -9320,7 +9431,7 @@
       </c>
       <c r="E11" s="18">
         <f>'Advanced Learning'!M8</f>
-        <v>0</v>
+        <v>0.48079055327641601</v>
       </c>
       <c r="F11" s="18">
         <f>'Advanced Learning'!N8</f>
@@ -9328,7 +9439,7 @@
       </c>
       <c r="G11" s="18">
         <f>'Advanced Learning'!O8</f>
-        <v>0</v>
+        <v>0.91746491571428568</v>
       </c>
       <c r="H11" s="18">
         <f>'Advanced Learning'!P8</f>
@@ -9381,7 +9492,7 @@
       </c>
       <c r="G12" s="18">
         <f>'Advanced Learning'!O9</f>
-        <v>0</v>
+        <v>0.96847132285714288</v>
       </c>
       <c r="H12" s="18">
         <f>'Advanced Learning'!P9</f>
@@ -9850,7 +9961,7 @@
       </c>
       <c r="E23" s="6">
         <f>'Advanced Learning'!M14</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="F23" s="6">
         <f>'Advanced Learning'!N14</f>
@@ -9858,7 +9969,7 @@
       </c>
       <c r="G23" s="6">
         <f>'Advanced Learning'!O14</f>
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="H23" s="6">
         <f>'Advanced Learning'!P14</f>
@@ -9903,7 +10014,7 @@
       </c>
       <c r="E24" s="9">
         <f>'Advanced Learning'!M15</f>
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="F24" s="9">
         <f>'Advanced Learning'!N15</f>
@@ -9911,7 +10022,7 @@
       </c>
       <c r="G24" s="9">
         <f>'Advanced Learning'!O15</f>
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="H24" s="9">
         <f>'Advanced Learning'!P15</f>
@@ -9956,7 +10067,7 @@
       </c>
       <c r="E25" s="9">
         <f>'Advanced Learning'!M16</f>
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="F25" s="9">
         <f>'Advanced Learning'!N16</f>
@@ -9964,7 +10075,7 @@
       </c>
       <c r="G25" s="9">
         <f>'Advanced Learning'!O16</f>
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="H25" s="9">
         <f>'Advanced Learning'!P16</f>
@@ -10017,7 +10128,7 @@
       </c>
       <c r="G26" s="9">
         <f>'Advanced Learning'!O17</f>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H26" s="9">
         <f>'Advanced Learning'!P17</f>
@@ -10486,7 +10597,7 @@
       </c>
       <c r="E37" s="6">
         <f>'Advanced Learning'!M22</f>
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="F37" s="6">
         <f>'Advanced Learning'!N22</f>
@@ -10494,7 +10605,7 @@
       </c>
       <c r="G37" s="6">
         <f>'Advanced Learning'!O22</f>
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="H37" s="6">
         <f>'Advanced Learning'!P22</f>
@@ -10539,7 +10650,7 @@
       </c>
       <c r="E38" s="9">
         <f>'Advanced Learning'!M23</f>
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="F38" s="9">
         <f>'Advanced Learning'!N23</f>
@@ -10547,7 +10658,7 @@
       </c>
       <c r="G38" s="9">
         <f>'Advanced Learning'!O23</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="H38" s="9">
         <f>'Advanced Learning'!P23</f>
@@ -10592,7 +10703,7 @@
       </c>
       <c r="E39" s="9">
         <f>'Advanced Learning'!M24</f>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="F39" s="9">
         <f>'Advanced Learning'!N24</f>
@@ -10600,7 +10711,7 @@
       </c>
       <c r="G39" s="9">
         <f>'Advanced Learning'!O24</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="H39" s="9">
         <f>'Advanced Learning'!P24</f>
@@ -10653,7 +10764,7 @@
       </c>
       <c r="G40" s="9">
         <f>'Advanced Learning'!O25</f>
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="H40" s="9">
         <f>'Advanced Learning'!P25</f>
@@ -11122,7 +11233,7 @@
       </c>
       <c r="E51" s="6">
         <f>'Advanced Learning'!M30</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="F51" s="6">
         <f>'Advanced Learning'!N30</f>
@@ -11130,7 +11241,7 @@
       </c>
       <c r="G51" s="6">
         <f>'Advanced Learning'!O30</f>
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="H51" s="6">
         <f>'Advanced Learning'!P30</f>
@@ -11175,7 +11286,7 @@
       </c>
       <c r="E52" s="9">
         <f>'Advanced Learning'!M31</f>
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="F52" s="9">
         <f>'Advanced Learning'!N31</f>
@@ -11183,7 +11294,7 @@
       </c>
       <c r="G52" s="9">
         <f>'Advanced Learning'!O31</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="H52" s="9">
         <f>'Advanced Learning'!P31</f>
@@ -11228,7 +11339,7 @@
       </c>
       <c r="E53" s="9">
         <f>'Advanced Learning'!M32</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="F53" s="9">
         <f>'Advanced Learning'!N32</f>
@@ -11236,7 +11347,7 @@
       </c>
       <c r="G53" s="9">
         <f>'Advanced Learning'!O32</f>
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="H53" s="9">
         <f>'Advanced Learning'!P32</f>
@@ -11289,7 +11400,7 @@
       </c>
       <c r="G54" s="9">
         <f>'Advanced Learning'!O33</f>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="H54" s="9">
         <f>'Advanced Learning'!P33</f>

</xml_diff>

<commit_message>
Finished Predictions and added LaTeX
</commit_message>
<xml_diff>
--- a/Classification Cont.xlsx
+++ b/Classification Cont.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Documents\SCHOOL\Towson\2018-2022 -- DSc - Computer Security\6_Fall 2018\COSC 757 - Data Mining\Assignments\Classification Competition - 11-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBBAFDE-8F7B-4FFD-9BA0-AD389C31B201}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996177B8-D450-425A-B864-A508478E4D92}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="86">
   <si>
     <t>TN</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Deep Networks</t>
   </si>
   <si>
-    <t>250-100-10-7</t>
-  </si>
-  <si>
     <t>250-100-10-7_32-16</t>
   </si>
   <si>
@@ -291,7 +288,7 @@
     <t>250-100-10-7_1-64-mult</t>
   </si>
   <si>
-    <t>250-100-10-7_RNN</t>
+    <t>500-250-100-10-7_32-16</t>
   </si>
 </sst>
 </file>
@@ -3327,8 +3324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6114,14 +6111,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -6202,23 +6202,23 @@
       </c>
       <c r="K5" s="27" t="str">
         <f>A13</f>
-        <v>FULL SET 2</v>
+        <v>Binary Only 1</v>
       </c>
       <c r="L5" s="27" t="str">
         <f>A21</f>
-        <v>Binary Only 1</v>
+        <v>Numeric Only 1</v>
       </c>
       <c r="M5" s="27" t="str">
         <f>A29</f>
-        <v>Numeric Only 1</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="N5" s="27" t="str">
         <f>A37</f>
-        <v>Numeric Only min-max 1</v>
-      </c>
-      <c r="O5" s="27" t="str">
+        <v>Deep Networks</v>
+      </c>
+      <c r="O5" s="27">
         <f>A45</f>
-        <v>Deep Networks</v>
+        <v>0</v>
       </c>
       <c r="P5" s="27">
         <f>A53</f>
@@ -6274,23 +6274,23 @@
       </c>
       <c r="K6" s="19">
         <f>B14</f>
-        <v>0.71413127841224</v>
+        <v>0.64724470562146497</v>
       </c>
       <c r="L6" s="19">
         <f>B22</f>
-        <v>0.64724470562146497</v>
+        <v>0.65996091584432803</v>
       </c>
       <c r="M6" s="19">
         <f>B30</f>
-        <v>0.65996091584432803</v>
+        <v>0.66467318993236502</v>
       </c>
       <c r="N6" s="19">
         <f>B38</f>
-        <v>0.66467318993236502</v>
+        <v>0.93721587857142852</v>
       </c>
       <c r="O6" s="19">
         <f>B46</f>
-        <v>0.93721587857142852</v>
+        <v>0</v>
       </c>
       <c r="P6" s="19">
         <f>B54</f>
@@ -6346,23 +6346,23 @@
       </c>
       <c r="K7" s="18">
         <f t="shared" ref="K7:K10" si="1">B15</f>
-        <v>0.85380862633507104</v>
+        <v>0.65204706730236095</v>
       </c>
       <c r="L7" s="18">
         <f t="shared" ref="L7:L10" si="2">B23</f>
-        <v>0.65204706730236095</v>
+        <v>0.48720756181394798</v>
       </c>
       <c r="M7" s="18">
         <f t="shared" ref="M7:M10" si="3">B31</f>
-        <v>0.48720756181394798</v>
+        <v>0.803803082381638</v>
       </c>
       <c r="N7" s="18">
         <f t="shared" ref="N7:N10" si="4">B39</f>
-        <v>0.803803082381638</v>
+        <v>0.89939790000000008</v>
       </c>
       <c r="O7" s="18">
         <f t="shared" ref="O7:O10" si="5">B47</f>
-        <v>0.89939790000000008</v>
+        <v>0</v>
       </c>
       <c r="P7" s="18">
         <f t="shared" ref="P7:P10" si="6">B55</f>
@@ -6418,23 +6418,23 @@
       </c>
       <c r="K8" s="18">
         <f t="shared" si="1"/>
-        <v>0.78661714158997598</v>
+        <v>0.65145803304135697</v>
       </c>
       <c r="L8" s="18">
         <f t="shared" si="2"/>
-        <v>0.65145803304135697</v>
+        <v>0.48079055327641601</v>
       </c>
       <c r="M8" s="18">
         <f t="shared" si="3"/>
-        <v>0.48079055327641601</v>
+        <v>0.74379088590752795</v>
       </c>
       <c r="N8" s="18">
         <f t="shared" si="4"/>
-        <v>0.74379088590752795</v>
+        <v>0.91746491571428568</v>
       </c>
       <c r="O8" s="18">
         <f t="shared" si="5"/>
-        <v>0.91746491571428568</v>
+        <v>0</v>
       </c>
       <c r="P8" s="18">
         <f t="shared" si="6"/>
@@ -6490,23 +6490,23 @@
       </c>
       <c r="K9" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="18">
+        <v>0.65094522674354105</v>
+      </c>
+      <c r="L9" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>0.65094522674354105</v>
+        <v>-</v>
       </c>
       <c r="M9" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.77036672580108601</v>
       </c>
       <c r="N9" s="18">
         <f t="shared" si="4"/>
-        <v>0.77036672580108601</v>
+        <v>0.96847132285714288</v>
       </c>
       <c r="O9" s="18">
         <f t="shared" si="5"/>
-        <v>0.96847132285714288</v>
+        <v>0</v>
       </c>
       <c r="P9" s="18">
         <f t="shared" si="6"/>
@@ -6565,19 +6565,19 @@
       </c>
       <c r="K10" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
+        <v>0.12628201574453901</v>
+      </c>
+      <c r="L10" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>0.12628201574453901</v>
+        <v>-</v>
       </c>
       <c r="M10" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.65524864175629205</v>
       </c>
       <c r="N10" s="18">
         <f t="shared" si="4"/>
-        <v>0.65524864175629205</v>
+        <v>0.95827459571428564</v>
       </c>
       <c r="O10" s="18">
         <f t="shared" si="5"/>
@@ -6640,19 +6640,19 @@
       </c>
       <c r="K11" s="17">
         <f t="shared" ref="K11" si="14">B19</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="17">
+        <v>0.61309457811287205</v>
+      </c>
+      <c r="L11" s="17" t="str">
         <f t="shared" ref="L11" si="15">B27</f>
-        <v>0.61309457811287205</v>
+        <v>-</v>
       </c>
       <c r="M11" s="17">
         <f t="shared" ref="M11" si="16">B35</f>
-        <v>0</v>
+        <v>0.61291440292715305</v>
       </c>
       <c r="N11" s="17">
         <f>B43</f>
-        <v>0.61291440292715305</v>
+        <v>0</v>
       </c>
       <c r="O11" s="17">
         <f t="shared" ref="O11" si="17">B51</f>
@@ -6699,7 +6699,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -6725,23 +6725,23 @@
       </c>
       <c r="K13" s="27" t="str">
         <f t="shared" ref="K13:U13" si="24">K5</f>
-        <v>FULL SET 2</v>
+        <v>Binary Only 1</v>
       </c>
       <c r="L13" s="27" t="str">
         <f t="shared" si="24"/>
-        <v>Binary Only 1</v>
+        <v>Numeric Only 1</v>
       </c>
       <c r="M13" s="27" t="str">
         <f t="shared" si="24"/>
-        <v>Numeric Only 1</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="N13" s="27" t="str">
         <f t="shared" si="24"/>
-        <v>Numeric Only min-max 1</v>
-      </c>
-      <c r="O13" s="27" t="str">
+        <v>Deep Networks</v>
+      </c>
+      <c r="O13" s="27">
         <f t="shared" si="24"/>
-        <v>Deep Networks</v>
+        <v>0</v>
       </c>
       <c r="P13" s="27">
         <f t="shared" si="24"/>
@@ -6773,16 +6773,16 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>0.71413127841224</v>
+        <v>0.64724470562146497</v>
       </c>
       <c r="C14">
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
       <c r="D14">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="E14">
-        <v>0.7</v>
+        <v>0.62</v>
       </c>
       <c r="F14" s="1">
         <v>144304</v>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="K14" s="19">
         <f>C14</f>
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
       <c r="L14" s="19">
         <f>C22</f>
@@ -6805,15 +6805,15 @@
       </c>
       <c r="M14" s="19">
         <f>C30</f>
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="N14" s="19">
         <f>C38</f>
-        <v>0.64</v>
+        <v>0.78</v>
       </c>
       <c r="O14" s="19">
         <f>C46</f>
-        <v>0.78</v>
+        <v>0</v>
       </c>
       <c r="P14" s="19">
         <f>C54</f>
@@ -6845,16 +6845,16 @@
         <v>28</v>
       </c>
       <c r="B15">
-        <v>0.85380862633507104</v>
+        <v>0.65204706730236095</v>
       </c>
       <c r="C15">
-        <v>0.85</v>
+        <v>0.64</v>
       </c>
       <c r="D15">
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="E15">
-        <v>0.85</v>
+        <v>0.63</v>
       </c>
       <c r="F15" s="1">
         <v>144304</v>
@@ -6869,23 +6869,23 @@
       </c>
       <c r="K15" s="18">
         <f t="shared" ref="K15:K18" si="27">C15</f>
-        <v>0.85</v>
+        <v>0.64</v>
       </c>
       <c r="L15" s="18">
         <f t="shared" ref="L15:L18" si="28">C23</f>
-        <v>0.64</v>
+        <v>0.24</v>
       </c>
       <c r="M15" s="18">
         <f t="shared" ref="M15:M18" si="29">C31</f>
-        <v>0.24</v>
+        <v>0.8</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" ref="N15:N18" si="30">C39</f>
-        <v>0.8</v>
+        <v>0.62</v>
       </c>
       <c r="O15" s="18">
         <f t="shared" ref="O15:O18" si="31">C47</f>
-        <v>0.62</v>
+        <v>0</v>
       </c>
       <c r="P15" s="18">
         <f t="shared" ref="P15:P18" si="32">C55</f>
@@ -6917,16 +6917,16 @@
         <v>29</v>
       </c>
       <c r="B16">
-        <v>0.78661714158997598</v>
+        <v>0.65145803304135697</v>
       </c>
       <c r="C16">
-        <v>0.78</v>
+        <v>0.64</v>
       </c>
       <c r="D16">
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
       <c r="E16">
-        <v>0.78</v>
+        <v>0.63</v>
       </c>
       <c r="F16" s="1">
         <v>144304</v>
@@ -6941,23 +6941,23 @@
       </c>
       <c r="K16" s="18">
         <f t="shared" si="27"/>
-        <v>0.78</v>
+        <v>0.64</v>
       </c>
       <c r="L16" s="18">
         <f t="shared" si="28"/>
-        <v>0.64</v>
+        <v>0.37</v>
       </c>
       <c r="M16" s="18">
         <f t="shared" si="29"/>
-        <v>0.37</v>
+        <v>0.74</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="30"/>
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="O16" s="18">
         <f t="shared" si="31"/>
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="P16" s="18">
         <f t="shared" si="32"/>
@@ -6988,6 +6988,18 @@
       <c r="A17" t="s">
         <v>30</v>
       </c>
+      <c r="B17">
+        <v>0.65094522674354105</v>
+      </c>
+      <c r="C17">
+        <v>0.64</v>
+      </c>
+      <c r="D17">
+        <v>0.65</v>
+      </c>
+      <c r="E17">
+        <v>0.63</v>
+      </c>
       <c r="F17" s="1">
         <v>144304</v>
       </c>
@@ -7001,23 +7013,23 @@
       </c>
       <c r="K17" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="18">
+        <v>0.64</v>
+      </c>
+      <c r="L17" s="18" t="str">
         <f t="shared" si="28"/>
-        <v>0.64</v>
+        <v>-</v>
       </c>
       <c r="M17" s="18">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="N17" s="18">
         <f t="shared" si="30"/>
-        <v>0.74</v>
+        <v>0.9</v>
       </c>
       <c r="O17" s="18">
         <f t="shared" si="31"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P17" s="18">
         <f t="shared" si="32"/>
@@ -7048,9 +7060,18 @@
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="B18">
+        <v>0.12628201574453901</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.12</v>
+      </c>
       <c r="F18" s="1">
         <v>144304</v>
       </c>
@@ -7064,19 +7085,19 @@
       </c>
       <c r="K18" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
+        <v>0.74</v>
+      </c>
+      <c r="L18" s="18" t="str">
         <f t="shared" si="28"/>
-        <v>0.74</v>
+        <v>-</v>
       </c>
       <c r="M18" s="18">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="N18" s="18">
         <f t="shared" si="30"/>
-        <v>0.64</v>
+        <v>0.84</v>
       </c>
       <c r="O18" s="18">
         <f t="shared" si="31"/>
@@ -7111,9 +7132,18 @@
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="B19">
+        <v>0.61309457811287205</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="F19" s="1">
         <v>144304</v>
       </c>
@@ -7127,19 +7157,19 @@
       </c>
       <c r="K19" s="17">
         <f t="shared" ref="K19" si="39">C19</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="17">
+        <v>0.62</v>
+      </c>
+      <c r="L19" s="17" t="str">
         <f t="shared" ref="L19" si="40">C27</f>
-        <v>0.62</v>
+        <v>-</v>
       </c>
       <c r="M19" s="17">
         <f t="shared" ref="M19" si="41">C35</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="N19" s="17">
         <f t="shared" ref="N19" si="42">C43</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="O19" s="17">
         <f t="shared" ref="O19" si="43">C51</f>
@@ -7186,7 +7216,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -7212,23 +7242,23 @@
       </c>
       <c r="K21" s="27" t="str">
         <f t="shared" ref="K21:U21" si="50">K5</f>
-        <v>FULL SET 2</v>
+        <v>Binary Only 1</v>
       </c>
       <c r="L21" s="27" t="str">
         <f t="shared" si="50"/>
-        <v>Binary Only 1</v>
+        <v>Numeric Only 1</v>
       </c>
       <c r="M21" s="27" t="str">
         <f t="shared" si="50"/>
-        <v>Numeric Only 1</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="N21" s="27" t="str">
         <f t="shared" si="50"/>
-        <v>Numeric Only min-max 1</v>
-      </c>
-      <c r="O21" s="27" t="str">
+        <v>Deep Networks</v>
+      </c>
+      <c r="O21" s="27">
         <f t="shared" si="50"/>
-        <v>Deep Networks</v>
+        <v>0</v>
       </c>
       <c r="P21" s="27">
         <f t="shared" si="50"/>
@@ -7260,16 +7290,16 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.64724470562146497</v>
+        <v>0.65996091584432803</v>
       </c>
       <c r="C22">
         <v>0.63</v>
       </c>
       <c r="D22">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="E22">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="F22" s="1">
         <v>144304</v>
@@ -7284,23 +7314,23 @@
       </c>
       <c r="K22" s="19">
         <f t="shared" ref="K22:K27" si="52">D14</f>
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="L22" s="19">
         <f>D22</f>
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="M22" s="19">
         <f>D30</f>
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="N22" s="19">
         <f>D38</f>
-        <v>0.65</v>
+        <v>0.77</v>
       </c>
       <c r="O22" s="19">
         <f>D46</f>
-        <v>0.77</v>
+        <v>0</v>
       </c>
       <c r="P22" s="19">
         <f>D54</f>
@@ -7332,16 +7362,16 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.65204706730236095</v>
+        <v>0.48720756181394798</v>
       </c>
       <c r="C23">
-        <v>0.64</v>
+        <v>0.24</v>
       </c>
       <c r="D23">
-        <v>0.65</v>
+        <v>0.49</v>
       </c>
       <c r="E23">
-        <v>0.63</v>
+        <v>0.32</v>
       </c>
       <c r="F23" s="1">
         <v>144304</v>
@@ -7356,23 +7386,23 @@
       </c>
       <c r="K23" s="18">
         <f t="shared" si="52"/>
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="L23" s="18">
         <f t="shared" ref="L23:L26" si="54">D23</f>
-        <v>0.65</v>
+        <v>0.49</v>
       </c>
       <c r="M23" s="18">
         <f t="shared" ref="M23:M26" si="55">D31</f>
-        <v>0.49</v>
+        <v>0.8</v>
       </c>
       <c r="N23" s="18">
         <f t="shared" ref="N23:N26" si="56">D39</f>
-        <v>0.8</v>
+        <v>0.63</v>
       </c>
       <c r="O23" s="18">
         <f t="shared" ref="O23:O26" si="57">D47</f>
-        <v>0.63</v>
+        <v>0</v>
       </c>
       <c r="P23" s="18">
         <f t="shared" ref="P23:P26" si="58">D55</f>
@@ -7404,16 +7434,16 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.65145803304135697</v>
+        <v>0.48079055327641601</v>
       </c>
       <c r="C24">
-        <v>0.64</v>
+        <v>0.37</v>
       </c>
       <c r="D24">
-        <v>0.65</v>
+        <v>0.48</v>
       </c>
       <c r="E24">
-        <v>0.63</v>
+        <v>0.33</v>
       </c>
       <c r="F24" s="1">
         <v>144304</v>
@@ -7428,23 +7458,23 @@
       </c>
       <c r="K24" s="18">
         <f t="shared" si="52"/>
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
       <c r="L24" s="18">
         <f t="shared" si="54"/>
-        <v>0.65</v>
+        <v>0.48</v>
       </c>
       <c r="M24" s="18">
         <f t="shared" si="55"/>
-        <v>0.48</v>
+        <v>0.74</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="56"/>
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="O24" s="18">
         <f t="shared" si="57"/>
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="P24" s="18">
         <f t="shared" si="58"/>
@@ -7475,17 +7505,17 @@
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
-        <v>0.65094522674354105</v>
-      </c>
-      <c r="C25">
-        <v>0.64</v>
-      </c>
-      <c r="D25">
-        <v>0.65</v>
-      </c>
-      <c r="E25">
-        <v>0.63</v>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>68</v>
       </c>
       <c r="F25" s="1">
         <v>144304</v>
@@ -7500,23 +7530,23 @@
       </c>
       <c r="K25" s="18">
         <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
+        <v>0.65</v>
+      </c>
+      <c r="L25" s="18" t="str">
         <f t="shared" si="54"/>
-        <v>0.65</v>
+        <v>-</v>
       </c>
       <c r="M25" s="18">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="N25" s="18">
         <f t="shared" si="56"/>
-        <v>0.74</v>
+        <v>0.88</v>
       </c>
       <c r="O25" s="18">
         <f t="shared" si="57"/>
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="P25" s="18">
         <f t="shared" si="58"/>
@@ -7547,17 +7577,17 @@
       <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26">
-        <v>0.12628201574453901</v>
-      </c>
-      <c r="C26">
-        <v>0.74</v>
-      </c>
-      <c r="D26">
-        <v>0.13</v>
-      </c>
-      <c r="E26">
-        <v>0.12</v>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
       </c>
       <c r="F26" s="1">
         <v>144304</v>
@@ -7572,19 +7602,19 @@
       </c>
       <c r="K26" s="18">
         <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="L26" s="18" t="str">
         <f t="shared" si="54"/>
-        <v>0.13</v>
+        <v>-</v>
       </c>
       <c r="M26" s="18">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="N26" s="18">
         <f t="shared" si="56"/>
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="O26" s="18">
         <f t="shared" si="57"/>
@@ -7619,17 +7649,17 @@
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27">
-        <v>0.61309457811287205</v>
-      </c>
-      <c r="C27">
-        <v>0.62</v>
-      </c>
-      <c r="D27">
-        <v>0.61</v>
-      </c>
-      <c r="E27">
-        <v>0.56999999999999995</v>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
       </c>
       <c r="F27" s="1">
         <v>144304</v>
@@ -7644,19 +7674,19 @@
       </c>
       <c r="K27" s="17">
         <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="17">
+        <v>0.61</v>
+      </c>
+      <c r="L27" s="17" t="str">
         <f t="shared" ref="L27" si="65">D27</f>
-        <v>0.61</v>
+        <v>-</v>
       </c>
       <c r="M27" s="17">
         <f t="shared" ref="M27" si="66">D35</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="N27" s="17">
         <f t="shared" ref="N27" si="67">D43</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="O27" s="17">
         <f t="shared" ref="O27" si="68">D51</f>
@@ -7703,7 +7733,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -7729,23 +7759,23 @@
       </c>
       <c r="K29" s="27" t="str">
         <f t="shared" ref="K29:U29" si="75">K5</f>
-        <v>FULL SET 2</v>
+        <v>Binary Only 1</v>
       </c>
       <c r="L29" s="27" t="str">
         <f t="shared" si="75"/>
-        <v>Binary Only 1</v>
+        <v>Numeric Only 1</v>
       </c>
       <c r="M29" s="27" t="str">
         <f t="shared" si="75"/>
-        <v>Numeric Only 1</v>
+        <v>Numeric Only min-max 1</v>
       </c>
       <c r="N29" s="27" t="str">
         <f t="shared" si="75"/>
-        <v>Numeric Only min-max 1</v>
-      </c>
-      <c r="O29" s="27" t="str">
+        <v>Deep Networks</v>
+      </c>
+      <c r="O29" s="27">
         <f t="shared" si="75"/>
-        <v>Deep Networks</v>
+        <v>0</v>
       </c>
       <c r="P29" s="27">
         <f t="shared" si="75"/>
@@ -7777,13 +7807,13 @@
         <v>27</v>
       </c>
       <c r="B30">
-        <v>0.65996091584432803</v>
+        <v>0.66467318993236502</v>
       </c>
       <c r="C30">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="D30">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="E30">
         <v>0.63</v>
@@ -7801,11 +7831,11 @@
       </c>
       <c r="K30" s="19">
         <f t="shared" ref="K30:K35" si="77">E14</f>
-        <v>0.7</v>
+        <v>0.62</v>
       </c>
       <c r="L30" s="19">
         <f t="shared" ref="L30:L35" si="78">E22</f>
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="M30" s="19">
         <f>E30</f>
@@ -7813,11 +7843,11 @@
       </c>
       <c r="N30" s="19">
         <f>E38</f>
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
       <c r="O30" s="19">
         <f>E46</f>
-        <v>0.76</v>
+        <v>0</v>
       </c>
       <c r="P30" s="19">
         <f>E54</f>
@@ -7849,16 +7879,16 @@
         <v>28</v>
       </c>
       <c r="B31">
-        <v>0.48720756181394798</v>
+        <v>0.803803082381638</v>
       </c>
       <c r="C31">
-        <v>0.24</v>
+        <v>0.8</v>
       </c>
       <c r="D31">
-        <v>0.49</v>
+        <v>0.8</v>
       </c>
       <c r="E31">
-        <v>0.32</v>
+        <v>0.8</v>
       </c>
       <c r="F31" s="1">
         <v>144304</v>
@@ -7873,23 +7903,23 @@
       </c>
       <c r="K31" s="18">
         <f t="shared" si="77"/>
-        <v>0.85</v>
+        <v>0.63</v>
       </c>
       <c r="L31" s="18">
         <f t="shared" si="78"/>
-        <v>0.63</v>
+        <v>0.32</v>
       </c>
       <c r="M31" s="18">
         <f t="shared" ref="M31:M34" si="80">E31</f>
-        <v>0.32</v>
+        <v>0.8</v>
       </c>
       <c r="N31" s="18">
         <f t="shared" ref="N31:N34" si="81">E39</f>
-        <v>0.8</v>
+        <v>0.61</v>
       </c>
       <c r="O31" s="18">
         <f t="shared" ref="O31:O34" si="82">E47</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="P31" s="18">
         <f t="shared" ref="P31:P34" si="83">E55</f>
@@ -7921,16 +7951,16 @@
         <v>29</v>
       </c>
       <c r="B32">
-        <v>0.48079055327641601</v>
+        <v>0.74379088590752795</v>
       </c>
       <c r="C32">
-        <v>0.37</v>
+        <v>0.74</v>
       </c>
       <c r="D32">
-        <v>0.48</v>
+        <v>0.74</v>
       </c>
       <c r="E32">
-        <v>0.33</v>
+        <v>0.74</v>
       </c>
       <c r="F32" s="1">
         <v>144304</v>
@@ -7945,23 +7975,23 @@
       </c>
       <c r="K32" s="18">
         <f t="shared" si="77"/>
-        <v>0.78</v>
+        <v>0.63</v>
       </c>
       <c r="L32" s="18">
         <f t="shared" si="78"/>
-        <v>0.63</v>
+        <v>0.33</v>
       </c>
       <c r="M32" s="18">
         <f t="shared" si="80"/>
-        <v>0.33</v>
+        <v>0.74</v>
       </c>
       <c r="N32" s="18">
         <f t="shared" si="81"/>
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="O32" s="18">
         <f t="shared" si="82"/>
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="P32" s="18">
         <f t="shared" si="83"/>
@@ -7992,6 +8022,18 @@
       <c r="A33" t="s">
         <v>30</v>
       </c>
+      <c r="B33">
+        <v>0.77036672580108601</v>
+      </c>
+      <c r="C33">
+        <v>0.74</v>
+      </c>
+      <c r="D33">
+        <v>0.74</v>
+      </c>
+      <c r="E33">
+        <v>0.74</v>
+      </c>
       <c r="F33" s="1">
         <v>144304</v>
       </c>
@@ -8005,23 +8047,23 @@
       </c>
       <c r="K33" s="18">
         <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="18">
+        <v>0.63</v>
+      </c>
+      <c r="L33" s="18" t="str">
         <f t="shared" si="78"/>
-        <v>0.63</v>
+        <v>-</v>
       </c>
       <c r="M33" s="18">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="N33" s="18">
         <f t="shared" si="81"/>
-        <v>0.74</v>
+        <v>0.89</v>
       </c>
       <c r="O33" s="18">
         <f t="shared" si="82"/>
-        <v>0.89</v>
+        <v>0</v>
       </c>
       <c r="P33" s="18">
         <f t="shared" si="83"/>
@@ -8052,6 +8094,18 @@
       <c r="A34" t="s">
         <v>31</v>
       </c>
+      <c r="B34">
+        <v>0.65524864175629205</v>
+      </c>
+      <c r="C34">
+        <v>0.64</v>
+      </c>
+      <c r="D34">
+        <v>0.65</v>
+      </c>
+      <c r="E34">
+        <v>0.64</v>
+      </c>
       <c r="F34" s="1">
         <v>144304</v>
       </c>
@@ -8065,19 +8119,19 @@
       </c>
       <c r="K34" s="18">
         <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="L34" s="18" t="str">
         <f t="shared" si="78"/>
-        <v>0.12</v>
+        <v>-</v>
       </c>
       <c r="M34" s="18">
         <f t="shared" si="80"/>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="N34" s="18">
         <f t="shared" si="81"/>
-        <v>0.64</v>
+        <v>0.84</v>
       </c>
       <c r="O34" s="18">
         <f t="shared" si="82"/>
@@ -8112,6 +8166,18 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
+      <c r="B35">
+        <v>0.61291440292715305</v>
+      </c>
+      <c r="C35">
+        <v>0.61</v>
+      </c>
+      <c r="D35">
+        <v>0.61</v>
+      </c>
+      <c r="E35">
+        <v>0.61</v>
+      </c>
       <c r="F35" s="1">
         <v>144304</v>
       </c>
@@ -8125,19 +8191,19 @@
       </c>
       <c r="K35" s="17">
         <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="17">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L35" s="17" t="str">
         <f t="shared" si="78"/>
-        <v>0.56999999999999995</v>
+        <v>-</v>
       </c>
       <c r="M35" s="17">
         <f t="shared" ref="M35" si="90">E35</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="N35" s="17">
         <f t="shared" ref="N35" si="91">E43</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="O35" s="17">
         <f t="shared" ref="O35" si="92">E51</f>
@@ -8170,7 +8236,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -8190,128 +8256,111 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="B38">
-        <v>0.66467318993236502</v>
+        <v>0.93721587857142852</v>
       </c>
       <c r="C38">
-        <v>0.64</v>
+        <v>0.78</v>
       </c>
       <c r="D38">
-        <v>0.65</v>
+        <v>0.77</v>
       </c>
       <c r="E38">
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
       <c r="F38" s="1">
-        <v>144304</v>
+        <v>120253</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="B39">
-        <v>0.803803082381638</v>
+        <v>0.89939790000000008</v>
       </c>
       <c r="C39">
-        <v>0.8</v>
+        <v>0.62</v>
       </c>
       <c r="D39">
-        <v>0.8</v>
+        <v>0.63</v>
       </c>
       <c r="E39">
-        <v>0.8</v>
+        <v>0.61</v>
       </c>
       <c r="F39" s="1">
-        <v>144304</v>
+        <v>120253</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="B40">
-        <v>0.74379088590752795</v>
+        <v>0.91746491571428568</v>
       </c>
       <c r="C40">
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="D40">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="E40">
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="F40" s="1">
-        <v>144304</v>
+        <v>120253</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="B41">
-        <v>0.77036672580108601</v>
+        <v>0.96847132285714288</v>
       </c>
       <c r="C41">
-        <v>0.74</v>
+        <v>0.9</v>
       </c>
       <c r="D41">
-        <v>0.74</v>
+        <v>0.88</v>
       </c>
       <c r="E41">
-        <v>0.74</v>
+        <v>0.89</v>
       </c>
       <c r="F41" s="1">
-        <v>144304</v>
+        <v>120253</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B42">
-        <v>0.65524864175629205</v>
+        <v>0.95827459571428564</v>
       </c>
       <c r="C42">
-        <v>0.64</v>
+        <v>0.84</v>
       </c>
       <c r="D42">
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="E42">
-        <v>0.64</v>
+        <v>0.84</v>
       </c>
       <c r="F42" s="1">
-        <v>144304</v>
+        <v>120253</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43">
-        <v>0.61291440292715305</v>
-      </c>
-      <c r="C43">
-        <v>0.61</v>
-      </c>
-      <c r="D43">
-        <v>0.61</v>
-      </c>
-      <c r="E43">
-        <v>0.61</v>
-      </c>
       <c r="F43" s="1">
-        <v>144304</v>
+        <v>120253</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" t="s">
         <v>6</v>
       </c>
@@ -8330,20 +8379,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46">
-        <f>AVERAGE(0.83687909, 0.81979017, 0.96844162, 0.99526694, 0.98501774, 0.97060373, 0.98451186)</f>
-        <v>0.93721587857142852</v>
-      </c>
-      <c r="C46">
-        <v>0.78</v>
-      </c>
-      <c r="D46">
-        <v>0.77</v>
-      </c>
-      <c r="E46">
-        <v>0.76</v>
+        <v>27</v>
       </c>
       <c r="F46">
         <v>120253</v>
@@ -8351,20 +8387,7 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47">
-        <f>AVERAGE(0.72299451, 0.69590587,0.95264858, 0.99526694,0.98354169, 0.97014636, 0.97528135)</f>
-        <v>0.89939790000000008</v>
-      </c>
-      <c r="C47">
-        <v>0.62</v>
-      </c>
-      <c r="D47">
-        <v>0.63</v>
-      </c>
-      <c r="E47">
-        <v>0.61</v>
+        <v>28</v>
       </c>
       <c r="F47">
         <v>120253</v>
@@ -8372,20 +8395,7 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48">
-        <f>AVERAGE(0.77954873, 0.76406752, 0.95583629, 0.99526694,0.98354169,0.97014636, 0.97384688)</f>
-        <v>0.91746491571428568</v>
-      </c>
-      <c r="C48">
-        <v>0.69</v>
-      </c>
-      <c r="D48">
-        <v>0.7</v>
-      </c>
-      <c r="E48">
-        <v>0.69</v>
+        <v>29</v>
       </c>
       <c r="F48">
         <v>120253</v>
@@ -8393,20 +8403,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49">
-        <f>AVERAGE(0.92409774,0.91172109,0.98151125,0.99745676,0.99081107,0.98283485, 0.9908665)</f>
-        <v>0.96847132285714288</v>
-      </c>
-      <c r="C49">
-        <v>0.9</v>
-      </c>
-      <c r="D49">
-        <v>0.88</v>
-      </c>
-      <c r="E49">
-        <v>0.89</v>
+        <v>30</v>
       </c>
       <c r="F49">
         <v>120253</v>
@@ -8414,7 +8411,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="F50">
         <v>120253</v>
@@ -8422,7 +8419,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="F51">
         <v>120253</v>
@@ -8979,7 +8976,7 @@
   <dimension ref="A3:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9317,23 +9314,23 @@
       </c>
       <c r="C9" s="19">
         <f>'Advanced Learning'!K6</f>
-        <v>0.71413127841224</v>
+        <v>0.64724470562146497</v>
       </c>
       <c r="D9" s="19">
         <f>'Advanced Learning'!L6</f>
-        <v>0.64724470562146497</v>
+        <v>0.65996091584432803</v>
       </c>
       <c r="E9" s="19">
         <f>'Advanced Learning'!M6</f>
-        <v>0.65996091584432803</v>
+        <v>0.66467318993236502</v>
       </c>
       <c r="F9" s="19">
         <f>'Advanced Learning'!N6</f>
-        <v>0.66467318993236502</v>
+        <v>0.93721587857142852</v>
       </c>
       <c r="G9" s="19">
         <f>'Advanced Learning'!O6</f>
-        <v>0.93721587857142852</v>
+        <v>0</v>
       </c>
       <c r="H9" s="19">
         <f>'Advanced Learning'!P6</f>
@@ -9370,23 +9367,23 @@
       </c>
       <c r="C10" s="18">
         <f>'Advanced Learning'!K7</f>
-        <v>0.85380862633507104</v>
+        <v>0.65204706730236095</v>
       </c>
       <c r="D10" s="18">
         <f>'Advanced Learning'!L7</f>
-        <v>0.65204706730236095</v>
+        <v>0.48720756181394798</v>
       </c>
       <c r="E10" s="18">
         <f>'Advanced Learning'!M7</f>
-        <v>0.48720756181394798</v>
+        <v>0.803803082381638</v>
       </c>
       <c r="F10" s="18">
         <f>'Advanced Learning'!N7</f>
-        <v>0.803803082381638</v>
+        <v>0.89939790000000008</v>
       </c>
       <c r="G10" s="18">
         <f>'Advanced Learning'!O7</f>
-        <v>0.89939790000000008</v>
+        <v>0</v>
       </c>
       <c r="H10" s="18">
         <f>'Advanced Learning'!P7</f>
@@ -9423,23 +9420,23 @@
       </c>
       <c r="C11" s="18">
         <f>'Advanced Learning'!K8</f>
-        <v>0.78661714158997598</v>
+        <v>0.65145803304135697</v>
       </c>
       <c r="D11" s="18">
         <f>'Advanced Learning'!L8</f>
-        <v>0.65145803304135697</v>
+        <v>0.48079055327641601</v>
       </c>
       <c r="E11" s="18">
         <f>'Advanced Learning'!M8</f>
-        <v>0.48079055327641601</v>
+        <v>0.74379088590752795</v>
       </c>
       <c r="F11" s="18">
         <f>'Advanced Learning'!N8</f>
-        <v>0.74379088590752795</v>
+        <v>0.91746491571428568</v>
       </c>
       <c r="G11" s="18">
         <f>'Advanced Learning'!O8</f>
-        <v>0.91746491571428568</v>
+        <v>0</v>
       </c>
       <c r="H11" s="18">
         <f>'Advanced Learning'!P8</f>
@@ -9476,23 +9473,23 @@
       </c>
       <c r="C12" s="18">
         <f>'Advanced Learning'!K9</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="18">
+        <v>0.65094522674354105</v>
+      </c>
+      <c r="D12" s="18" t="str">
         <f>'Advanced Learning'!L9</f>
-        <v>0.65094522674354105</v>
+        <v>-</v>
       </c>
       <c r="E12" s="18">
         <f>'Advanced Learning'!M9</f>
-        <v>0</v>
+        <v>0.77036672580108601</v>
       </c>
       <c r="F12" s="18">
         <f>'Advanced Learning'!N9</f>
-        <v>0.77036672580108601</v>
+        <v>0.96847132285714288</v>
       </c>
       <c r="G12" s="18">
         <f>'Advanced Learning'!O9</f>
-        <v>0.96847132285714288</v>
+        <v>0</v>
       </c>
       <c r="H12" s="18">
         <f>'Advanced Learning'!P9</f>
@@ -9529,19 +9526,19 @@
       </c>
       <c r="C13" s="18">
         <f>'Advanced Learning'!K10</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="18">
+        <v>0.12628201574453901</v>
+      </c>
+      <c r="D13" s="18" t="str">
         <f>'Advanced Learning'!L10</f>
-        <v>0.12628201574453901</v>
+        <v>-</v>
       </c>
       <c r="E13" s="18">
         <f>'Advanced Learning'!M10</f>
-        <v>0</v>
+        <v>0.65524864175629205</v>
       </c>
       <c r="F13" s="18">
         <f>'Advanced Learning'!N10</f>
-        <v>0.65524864175629205</v>
+        <v>0.95827459571428564</v>
       </c>
       <c r="G13" s="18">
         <f>'Advanced Learning'!O10</f>
@@ -9582,19 +9579,19 @@
       </c>
       <c r="C14" s="17">
         <f>'Advanced Learning'!K11</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="17">
+        <v>0.61309457811287205</v>
+      </c>
+      <c r="D14" s="17" t="str">
         <f>'Advanced Learning'!L11</f>
-        <v>0.61309457811287205</v>
+        <v>-</v>
       </c>
       <c r="E14" s="17">
         <f>'Advanced Learning'!M11</f>
-        <v>0</v>
+        <v>0.61291440292715305</v>
       </c>
       <c r="F14" s="17">
         <f>'Advanced Learning'!N11</f>
-        <v>0.61291440292715305</v>
+        <v>0</v>
       </c>
       <c r="G14" s="17">
         <f>'Advanced Learning'!O11</f>
@@ -9953,7 +9950,7 @@
       </c>
       <c r="C23" s="6">
         <f>'Advanced Learning'!K14</f>
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
       <c r="D23" s="6">
         <f>'Advanced Learning'!L14</f>
@@ -9961,15 +9958,15 @@
       </c>
       <c r="E23" s="6">
         <f>'Advanced Learning'!M14</f>
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="F23" s="6">
         <f>'Advanced Learning'!N14</f>
-        <v>0.64</v>
+        <v>0.78</v>
       </c>
       <c r="G23" s="6">
         <f>'Advanced Learning'!O14</f>
-        <v>0.78</v>
+        <v>0</v>
       </c>
       <c r="H23" s="6">
         <f>'Advanced Learning'!P14</f>
@@ -10006,23 +10003,23 @@
       </c>
       <c r="C24" s="9">
         <f>'Advanced Learning'!K15</f>
-        <v>0.85</v>
+        <v>0.64</v>
       </c>
       <c r="D24" s="9">
         <f>'Advanced Learning'!L15</f>
-        <v>0.64</v>
+        <v>0.24</v>
       </c>
       <c r="E24" s="9">
         <f>'Advanced Learning'!M15</f>
-        <v>0.24</v>
+        <v>0.8</v>
       </c>
       <c r="F24" s="9">
         <f>'Advanced Learning'!N15</f>
-        <v>0.8</v>
+        <v>0.62</v>
       </c>
       <c r="G24" s="9">
         <f>'Advanced Learning'!O15</f>
-        <v>0.62</v>
+        <v>0</v>
       </c>
       <c r="H24" s="9">
         <f>'Advanced Learning'!P15</f>
@@ -10059,23 +10056,23 @@
       </c>
       <c r="C25" s="9">
         <f>'Advanced Learning'!K16</f>
-        <v>0.78</v>
+        <v>0.64</v>
       </c>
       <c r="D25" s="9">
         <f>'Advanced Learning'!L16</f>
-        <v>0.64</v>
+        <v>0.37</v>
       </c>
       <c r="E25" s="9">
         <f>'Advanced Learning'!M16</f>
-        <v>0.37</v>
+        <v>0.74</v>
       </c>
       <c r="F25" s="9">
         <f>'Advanced Learning'!N16</f>
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="G25" s="9">
         <f>'Advanced Learning'!O16</f>
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="H25" s="9">
         <f>'Advanced Learning'!P16</f>
@@ -10112,23 +10109,23 @@
       </c>
       <c r="C26" s="9">
         <f>'Advanced Learning'!K17</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="D26" s="9" t="str">
         <f>'Advanced Learning'!L17</f>
-        <v>0.64</v>
+        <v>-</v>
       </c>
       <c r="E26" s="9">
         <f>'Advanced Learning'!M17</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="F26" s="9">
         <f>'Advanced Learning'!N17</f>
-        <v>0.74</v>
+        <v>0.9</v>
       </c>
       <c r="G26" s="9">
         <f>'Advanced Learning'!O17</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="H26" s="9">
         <f>'Advanced Learning'!P17</f>
@@ -10165,19 +10162,19 @@
       </c>
       <c r="C27" s="9">
         <f>'Advanced Learning'!K18</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="D27" s="9" t="str">
         <f>'Advanced Learning'!L18</f>
-        <v>0.74</v>
+        <v>-</v>
       </c>
       <c r="E27" s="9">
         <f>'Advanced Learning'!M18</f>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="F27" s="9">
         <f>'Advanced Learning'!N18</f>
-        <v>0.64</v>
+        <v>0.84</v>
       </c>
       <c r="G27" s="9">
         <f>'Advanced Learning'!O18</f>
@@ -10218,19 +10215,19 @@
       </c>
       <c r="C28" s="12">
         <f>'Advanced Learning'!K19</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="12">
+        <v>0.62</v>
+      </c>
+      <c r="D28" s="12" t="str">
         <f>'Advanced Learning'!L19</f>
-        <v>0.62</v>
+        <v>-</v>
       </c>
       <c r="E28" s="12">
         <f>'Advanced Learning'!M19</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="F28" s="12">
         <f>'Advanced Learning'!N19</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="G28" s="12">
         <f>'Advanced Learning'!O19</f>
@@ -10589,23 +10586,23 @@
       </c>
       <c r="C37" s="6">
         <f>'Advanced Learning'!K22</f>
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="D37" s="6">
         <f>'Advanced Learning'!L22</f>
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="E37" s="6">
         <f>'Advanced Learning'!M22</f>
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="F37" s="6">
         <f>'Advanced Learning'!N22</f>
-        <v>0.65</v>
+        <v>0.77</v>
       </c>
       <c r="G37" s="6">
         <f>'Advanced Learning'!O22</f>
-        <v>0.77</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6">
         <f>'Advanced Learning'!P22</f>
@@ -10642,23 +10639,23 @@
       </c>
       <c r="C38" s="9">
         <f>'Advanced Learning'!K23</f>
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="D38" s="9">
         <f>'Advanced Learning'!L23</f>
-        <v>0.65</v>
+        <v>0.49</v>
       </c>
       <c r="E38" s="9">
         <f>'Advanced Learning'!M23</f>
-        <v>0.49</v>
+        <v>0.8</v>
       </c>
       <c r="F38" s="9">
         <f>'Advanced Learning'!N23</f>
-        <v>0.8</v>
+        <v>0.63</v>
       </c>
       <c r="G38" s="9">
         <f>'Advanced Learning'!O23</f>
-        <v>0.63</v>
+        <v>0</v>
       </c>
       <c r="H38" s="9">
         <f>'Advanced Learning'!P23</f>
@@ -10695,23 +10692,23 @@
       </c>
       <c r="C39" s="9">
         <f>'Advanced Learning'!K24</f>
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
       <c r="D39" s="9">
         <f>'Advanced Learning'!L24</f>
-        <v>0.65</v>
+        <v>0.48</v>
       </c>
       <c r="E39" s="9">
         <f>'Advanced Learning'!M24</f>
-        <v>0.48</v>
+        <v>0.74</v>
       </c>
       <c r="F39" s="9">
         <f>'Advanced Learning'!N24</f>
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="G39" s="9">
         <f>'Advanced Learning'!O24</f>
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="H39" s="9">
         <f>'Advanced Learning'!P24</f>
@@ -10748,23 +10745,23 @@
       </c>
       <c r="C40" s="9">
         <f>'Advanced Learning'!K25</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="D40" s="9" t="str">
         <f>'Advanced Learning'!L25</f>
-        <v>0.65</v>
+        <v>-</v>
       </c>
       <c r="E40" s="9">
         <f>'Advanced Learning'!M25</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="F40" s="9">
         <f>'Advanced Learning'!N25</f>
-        <v>0.74</v>
+        <v>0.88</v>
       </c>
       <c r="G40" s="9">
         <f>'Advanced Learning'!O25</f>
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="H40" s="9">
         <f>'Advanced Learning'!P25</f>
@@ -10801,19 +10798,19 @@
       </c>
       <c r="C41" s="9">
         <f>'Advanced Learning'!K26</f>
-        <v>0</v>
-      </c>
-      <c r="D41" s="9">
+        <v>0.13</v>
+      </c>
+      <c r="D41" s="9" t="str">
         <f>'Advanced Learning'!L26</f>
-        <v>0.13</v>
+        <v>-</v>
       </c>
       <c r="E41" s="9">
         <f>'Advanced Learning'!M26</f>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="F41" s="9">
         <f>'Advanced Learning'!N26</f>
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="G41" s="9">
         <f>'Advanced Learning'!O26</f>
@@ -10854,19 +10851,19 @@
       </c>
       <c r="C42" s="12">
         <f>'Advanced Learning'!K27</f>
-        <v>0</v>
-      </c>
-      <c r="D42" s="12">
+        <v>0.61</v>
+      </c>
+      <c r="D42" s="12" t="str">
         <f>'Advanced Learning'!L27</f>
-        <v>0.61</v>
+        <v>-</v>
       </c>
       <c r="E42" s="12">
         <f>'Advanced Learning'!M27</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="F42" s="12">
         <f>'Advanced Learning'!N27</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="G42" s="12">
         <f>'Advanced Learning'!O27</f>
@@ -11225,11 +11222,11 @@
       </c>
       <c r="C51" s="6">
         <f>'Advanced Learning'!K30</f>
-        <v>0.7</v>
+        <v>0.62</v>
       </c>
       <c r="D51" s="6">
         <f>'Advanced Learning'!L30</f>
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="E51" s="6">
         <f>'Advanced Learning'!M30</f>
@@ -11237,11 +11234,11 @@
       </c>
       <c r="F51" s="6">
         <f>'Advanced Learning'!N30</f>
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
       <c r="G51" s="6">
         <f>'Advanced Learning'!O30</f>
-        <v>0.76</v>
+        <v>0</v>
       </c>
       <c r="H51" s="6">
         <f>'Advanced Learning'!P30</f>
@@ -11278,23 +11275,23 @@
       </c>
       <c r="C52" s="9">
         <f>'Advanced Learning'!K31</f>
-        <v>0.85</v>
+        <v>0.63</v>
       </c>
       <c r="D52" s="9">
         <f>'Advanced Learning'!L31</f>
-        <v>0.63</v>
+        <v>0.32</v>
       </c>
       <c r="E52" s="9">
         <f>'Advanced Learning'!M31</f>
-        <v>0.32</v>
+        <v>0.8</v>
       </c>
       <c r="F52" s="9">
         <f>'Advanced Learning'!N31</f>
-        <v>0.8</v>
+        <v>0.61</v>
       </c>
       <c r="G52" s="9">
         <f>'Advanced Learning'!O31</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="H52" s="9">
         <f>'Advanced Learning'!P31</f>
@@ -11331,23 +11328,23 @@
       </c>
       <c r="C53" s="9">
         <f>'Advanced Learning'!K32</f>
-        <v>0.78</v>
+        <v>0.63</v>
       </c>
       <c r="D53" s="9">
         <f>'Advanced Learning'!L32</f>
-        <v>0.63</v>
+        <v>0.33</v>
       </c>
       <c r="E53" s="9">
         <f>'Advanced Learning'!M32</f>
-        <v>0.33</v>
+        <v>0.74</v>
       </c>
       <c r="F53" s="9">
         <f>'Advanced Learning'!N32</f>
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="G53" s="9">
         <f>'Advanced Learning'!O32</f>
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="H53" s="9">
         <f>'Advanced Learning'!P32</f>
@@ -11384,23 +11381,23 @@
       </c>
       <c r="C54" s="9">
         <f>'Advanced Learning'!K33</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="D54" s="9" t="str">
         <f>'Advanced Learning'!L33</f>
-        <v>0.63</v>
+        <v>-</v>
       </c>
       <c r="E54" s="9">
         <f>'Advanced Learning'!M33</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="F54" s="9">
         <f>'Advanced Learning'!N33</f>
-        <v>0.74</v>
+        <v>0.89</v>
       </c>
       <c r="G54" s="9">
         <f>'Advanced Learning'!O33</f>
-        <v>0.89</v>
+        <v>0</v>
       </c>
       <c r="H54" s="9">
         <f>'Advanced Learning'!P33</f>
@@ -11437,19 +11434,19 @@
       </c>
       <c r="C55" s="9">
         <f>'Advanced Learning'!K34</f>
-        <v>0</v>
-      </c>
-      <c r="D55" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="D55" s="9" t="str">
         <f>'Advanced Learning'!L34</f>
-        <v>0.12</v>
+        <v>-</v>
       </c>
       <c r="E55" s="9">
         <f>'Advanced Learning'!M34</f>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="F55" s="9">
         <f>'Advanced Learning'!N34</f>
-        <v>0.64</v>
+        <v>0.84</v>
       </c>
       <c r="G55" s="9">
         <f>'Advanced Learning'!O34</f>
@@ -11490,19 +11487,19 @@
       </c>
       <c r="C56" s="12">
         <f>'Advanced Learning'!K35</f>
-        <v>0</v>
-      </c>
-      <c r="D56" s="12">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D56" s="12" t="str">
         <f>'Advanced Learning'!L35</f>
-        <v>0.56999999999999995</v>
+        <v>-</v>
       </c>
       <c r="E56" s="12">
         <f>'Advanced Learning'!M35</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="F56" s="12">
         <f>'Advanced Learning'!N35</f>
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="G56" s="12">
         <f>'Advanced Learning'!O35</f>

</xml_diff>